<commit_message>
Get data from 'Data' sheet if no source data is given
Close #56
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDA631B-7403-4BE0-827A-DE8B0B923A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2107646-7827-4C18-B20C-DCD14C80C28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="31800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17265" yWindow="3315" windowWidth="23220" windowHeight="12855" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
     <sheet name="Variables" sheetId="1" r:id="rId2"/>
     <sheet name="Codelists" sheetId="3" r:id="rId3"/>
+    <sheet name="Data" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="128">
   <si>
     <t>type</t>
   </si>
@@ -403,6 +404,9 @@
   </si>
   <si>
     <t>en_code_label</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1488,4 +1492,1210 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
+  <dimension ref="A1:D85"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2">
+        <v>2018</v>
+      </c>
+      <c r="D2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3">
+        <v>2019</v>
+      </c>
+      <c r="D3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4">
+        <v>2020</v>
+      </c>
+      <c r="D4">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5">
+        <v>2021</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>2018</v>
+      </c>
+      <c r="D6">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>2019</v>
+      </c>
+      <c r="D7">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8">
+        <v>2020</v>
+      </c>
+      <c r="D8">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>2021</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10">
+        <v>2018</v>
+      </c>
+      <c r="D10">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11">
+        <v>2019</v>
+      </c>
+      <c r="D11">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12">
+        <v>2020</v>
+      </c>
+      <c r="D12">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13">
+        <v>2021</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14">
+        <v>2018</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15">
+        <v>2019</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16">
+        <v>2020</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17">
+        <v>2021</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18">
+        <v>2018</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>2019</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>2020</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>2021</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>2018</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <v>2019</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24">
+        <v>2020</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25">
+        <v>2021</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26">
+        <v>2018</v>
+      </c>
+      <c r="D26">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27">
+        <v>2019</v>
+      </c>
+      <c r="D27">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28">
+        <v>2020</v>
+      </c>
+      <c r="D28">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29">
+        <v>2021</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30">
+        <v>2018</v>
+      </c>
+      <c r="D30">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31">
+        <v>2019</v>
+      </c>
+      <c r="D31">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32">
+        <v>2020</v>
+      </c>
+      <c r="D32">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33">
+        <v>2021</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34">
+        <v>2018</v>
+      </c>
+      <c r="D34">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>2019</v>
+      </c>
+      <c r="D35">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36">
+        <v>2020</v>
+      </c>
+      <c r="D36">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37">
+        <v>2021</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38">
+        <v>2018</v>
+      </c>
+      <c r="D38">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39">
+        <v>2019</v>
+      </c>
+      <c r="D39">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40">
+        <v>2020</v>
+      </c>
+      <c r="D40">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41">
+        <v>2021</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42">
+        <v>2018</v>
+      </c>
+      <c r="D42">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>2019</v>
+      </c>
+      <c r="D43">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>2020</v>
+      </c>
+      <c r="D44">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45">
+        <v>2021</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46">
+        <v>2018</v>
+      </c>
+      <c r="D46">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47">
+        <v>2019</v>
+      </c>
+      <c r="D47">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48">
+        <v>2020</v>
+      </c>
+      <c r="D48">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49">
+        <v>2021</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50">
+        <v>2018</v>
+      </c>
+      <c r="D50">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51">
+        <v>2019</v>
+      </c>
+      <c r="D51">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52">
+        <v>2020</v>
+      </c>
+      <c r="D52">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53">
+        <v>2021</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54">
+        <v>2018</v>
+      </c>
+      <c r="D54">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55">
+        <v>2019</v>
+      </c>
+      <c r="D55">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56">
+        <v>2020</v>
+      </c>
+      <c r="D56">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57">
+        <v>2021</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58">
+        <v>2018</v>
+      </c>
+      <c r="D58">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59">
+        <v>2019</v>
+      </c>
+      <c r="D59">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60">
+        <v>2020</v>
+      </c>
+      <c r="D60">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61">
+        <v>2021</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62">
+        <v>2018</v>
+      </c>
+      <c r="D62">
+        <v>24461</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63">
+        <v>2019</v>
+      </c>
+      <c r="D63">
+        <v>24782</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>86</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64">
+        <v>2020</v>
+      </c>
+      <c r="D64">
+        <v>25157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65">
+        <v>2021</v>
+      </c>
+      <c r="D65">
+        <v>25525</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66">
+        <v>2018</v>
+      </c>
+      <c r="D66">
+        <v>26003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67">
+        <v>2019</v>
+      </c>
+      <c r="D67">
+        <v>26496</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68">
+        <v>2020</v>
+      </c>
+      <c r="D68">
+        <v>26952</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69">
+        <v>2021</v>
+      </c>
+      <c r="D69">
+        <v>27384</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70">
+        <v>2018</v>
+      </c>
+      <c r="D70">
+        <v>50464</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71">
+        <v>2019</v>
+      </c>
+      <c r="D71">
+        <v>51278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72">
+        <v>2020</v>
+      </c>
+      <c r="D72">
+        <v>52109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73" t="s">
+        <v>41</v>
+      </c>
+      <c r="C73">
+        <v>2021</v>
+      </c>
+      <c r="D73">
+        <v>52909</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" t="s">
+        <v>127</v>
+      </c>
+      <c r="C74">
+        <v>2018</v>
+      </c>
+      <c r="D74">
+        <v>24782</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75">
+        <v>2019</v>
+      </c>
+      <c r="D75">
+        <v>25157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76" t="s">
+        <v>127</v>
+      </c>
+      <c r="C76">
+        <v>2020</v>
+      </c>
+      <c r="D76">
+        <v>25525</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77">
+        <v>2021</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" t="s">
+        <v>42</v>
+      </c>
+      <c r="C78">
+        <v>2018</v>
+      </c>
+      <c r="D78">
+        <v>26496</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79">
+        <v>2019</v>
+      </c>
+      <c r="D79">
+        <v>26952</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" t="s">
+        <v>42</v>
+      </c>
+      <c r="C80">
+        <v>2020</v>
+      </c>
+      <c r="D80">
+        <v>27384</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" t="s">
+        <v>42</v>
+      </c>
+      <c r="C81">
+        <v>2021</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82" t="s">
+        <v>41</v>
+      </c>
+      <c r="C82">
+        <v>2018</v>
+      </c>
+      <c r="D82">
+        <v>51278</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C83">
+        <v>2019</v>
+      </c>
+      <c r="D83">
+        <v>52109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84">
+        <v>2020</v>
+      </c>
+      <c r="D84">
+        <v>52909</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" t="s">
+        <v>41</v>
+      </c>
+      <c r="C85">
+        <v>2021</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert changes in FOTEST
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E77C5D-CC8F-4CD2-A542-1D7191C96677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2107646-7827-4C18-B20C-DCD14C80C28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="16995" windowHeight="31785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17265" yWindow="3315" windowWidth="23220" windowHeight="12855" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -1285,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1498,7 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix mistake in FOTEST metadata
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2107646-7827-4C18-B20C-DCD14C80C28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6096C0ED-2C6B-4E07-95F1-A08343F99294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17265" yWindow="3315" windowWidth="23220" windowHeight="12855" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="615" windowWidth="16995" windowHeight="31785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="127">
   <si>
     <t>type</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>K</t>
   </si>
   <si>
     <t>20210211 09:00</t>
@@ -835,15 +832,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="4">
         <v>2000</v>
@@ -851,34 +848,34 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -891,26 +888,26 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1">
@@ -918,12 +915,12 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -939,7 +936,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -955,7 +952,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -971,7 +968,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -979,7 +976,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -987,7 +984,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
         <v>27</v>
@@ -995,10 +992,10 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1006,12 +1003,12 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
@@ -1019,7 +1016,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25" t="s">
         <v>29</v>
@@ -1027,23 +1024,23 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1051,7 +1048,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1059,10 +1056,10 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1070,15 +1067,15 @@
         <v>19</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
         <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1115,34 +1112,34 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>3</v>
@@ -1182,39 +1179,39 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1246,7 +1243,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1285,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1300,7 +1297,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>8</v>
@@ -1309,140 +1306,140 @@
         <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>86</v>
-      </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>41</v>
@@ -1456,10 +1453,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>42</v>
@@ -1473,13 +1470,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -1498,7 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1506,10 +1503,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>30</v>
@@ -1520,10 +1517,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2">
         <v>2018</v>
@@ -1534,10 +1531,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3">
         <v>2019</v>
@@ -1548,10 +1545,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4">
         <v>2020</v>
@@ -1562,10 +1559,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5">
         <v>2021</v>
@@ -1576,7 +1573,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -1590,7 +1587,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1604,7 +1601,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1618,7 +1615,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
@@ -1632,7 +1629,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
@@ -1646,7 +1643,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
@@ -1660,7 +1657,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>41</v>
@@ -1674,7 +1671,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
@@ -1688,10 +1685,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14">
         <v>2018</v>
@@ -1702,10 +1699,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C15">
         <v>2019</v>
@@ -1716,10 +1713,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16">
         <v>2020</v>
@@ -1730,10 +1727,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17">
         <v>2021</v>
@@ -1744,7 +1741,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
@@ -1758,7 +1755,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
         <v>42</v>
@@ -1772,7 +1769,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
         <v>42</v>
@@ -1786,7 +1783,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
@@ -1800,7 +1797,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
@@ -1814,7 +1811,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
@@ -1828,7 +1825,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
@@ -1842,7 +1839,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
         <v>41</v>
@@ -1856,10 +1853,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C26">
         <v>2018</v>
@@ -1870,10 +1867,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C27">
         <v>2019</v>
@@ -1884,10 +1881,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28">
         <v>2020</v>
@@ -1898,10 +1895,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29">
         <v>2021</v>
@@ -1912,7 +1909,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
         <v>42</v>
@@ -1926,7 +1923,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
         <v>42</v>
@@ -1940,7 +1937,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
         <v>42</v>
@@ -1954,7 +1951,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
         <v>42</v>
@@ -1968,7 +1965,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
         <v>41</v>
@@ -1982,7 +1979,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
         <v>41</v>
@@ -1996,7 +1993,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
         <v>41</v>
@@ -2010,7 +2007,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
         <v>41</v>
@@ -2024,10 +2021,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C38">
         <v>2018</v>
@@ -2038,10 +2035,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39">
         <v>2019</v>
@@ -2052,10 +2049,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C40">
         <v>2020</v>
@@ -2066,10 +2063,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C41">
         <v>2021</v>
@@ -2080,7 +2077,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
@@ -2094,7 +2091,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
@@ -2108,7 +2105,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
@@ -2122,7 +2119,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
         <v>42</v>
@@ -2136,7 +2133,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
         <v>41</v>
@@ -2150,7 +2147,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
         <v>41</v>
@@ -2164,7 +2161,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
         <v>41</v>
@@ -2178,7 +2175,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
         <v>41</v>
@@ -2192,10 +2189,10 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C50">
         <v>2018</v>
@@ -2206,10 +2203,10 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C51">
         <v>2019</v>
@@ -2220,10 +2217,10 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C52">
         <v>2020</v>
@@ -2234,10 +2231,10 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C53">
         <v>2021</v>
@@ -2248,7 +2245,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
         <v>42</v>
@@ -2262,7 +2259,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
         <v>42</v>
@@ -2276,7 +2273,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
         <v>42</v>
@@ -2290,7 +2287,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s">
         <v>42</v>
@@ -2304,7 +2301,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
         <v>41</v>
@@ -2318,7 +2315,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
         <v>41</v>
@@ -2332,7 +2329,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
         <v>41</v>
@@ -2346,7 +2343,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
         <v>41</v>
@@ -2360,10 +2357,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C62">
         <v>2018</v>
@@ -2374,10 +2371,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C63">
         <v>2019</v>
@@ -2388,10 +2385,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C64">
         <v>2020</v>
@@ -2402,10 +2399,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C65">
         <v>2021</v>
@@ -2416,7 +2413,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B66" t="s">
         <v>42</v>
@@ -2430,7 +2427,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
         <v>42</v>
@@ -2444,7 +2441,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
         <v>42</v>
@@ -2458,7 +2455,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B69" t="s">
         <v>42</v>
@@ -2472,7 +2469,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70" t="s">
         <v>41</v>
@@ -2486,7 +2483,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B71" t="s">
         <v>41</v>
@@ -2500,7 +2497,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
         <v>41</v>
@@ -2514,7 +2511,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
         <v>41</v>
@@ -2528,10 +2525,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B74" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C74">
         <v>2018</v>
@@ -2542,10 +2539,10 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C75">
         <v>2019</v>
@@ -2556,10 +2553,10 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B76" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C76">
         <v>2020</v>
@@ -2570,10 +2567,10 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C77">
         <v>2021</v>
@@ -2584,7 +2581,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B78" t="s">
         <v>42</v>
@@ -2598,7 +2595,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B79" t="s">
         <v>42</v>
@@ -2612,7 +2609,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B80" t="s">
         <v>42</v>
@@ -2626,7 +2623,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" t="s">
         <v>42</v>
@@ -2640,7 +2637,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B82" t="s">
         <v>41</v>
@@ -2654,7 +2651,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B83" t="s">
         <v>41</v>
@@ -2668,7 +2665,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" t="s">
         <v>41</v>
@@ -2682,7 +2679,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B85" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Add quaters to FOTEST and remove time_quater example
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6096C0ED-2C6B-4E07-95F1-A08343F99294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699A3483-62AD-4871-95E2-5634DBD21323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="615" windowWidth="16995" windowHeight="31785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21510" yWindow="4215" windowWidth="23730" windowHeight="20625" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="131">
   <si>
     <t>type</t>
   </si>
@@ -404,6 +404,18 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>2000Q1</t>
+  </si>
+  <si>
+    <t>2000Q2</t>
+  </si>
+  <si>
+    <t>2000Q3</t>
+  </si>
+  <si>
+    <t>2000Q4</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1495,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1522,8 +1534,8 @@
       <c r="B2" t="s">
         <v>126</v>
       </c>
-      <c r="C2">
-        <v>2018</v>
+      <c r="C2" t="s">
+        <v>127</v>
       </c>
       <c r="D2">
         <v>338</v>
@@ -1536,8 +1548,8 @@
       <c r="B3" t="s">
         <v>126</v>
       </c>
-      <c r="C3">
-        <v>2019</v>
+      <c r="C3" t="s">
+        <v>128</v>
       </c>
       <c r="D3">
         <v>340</v>
@@ -1550,8 +1562,8 @@
       <c r="B4" t="s">
         <v>126</v>
       </c>
-      <c r="C4">
-        <v>2020</v>
+      <c r="C4" t="s">
+        <v>129</v>
       </c>
       <c r="D4">
         <v>310</v>
@@ -1564,8 +1576,8 @@
       <c r="B5" t="s">
         <v>126</v>
       </c>
-      <c r="C5">
-        <v>2021</v>
+      <c r="C5" t="s">
+        <v>130</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1578,8 +1590,8 @@
       <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C6">
-        <v>2018</v>
+      <c r="C6" t="s">
+        <v>127</v>
       </c>
       <c r="D6">
         <v>346</v>
@@ -1592,8 +1604,8 @@
       <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7">
-        <v>2019</v>
+      <c r="C7" t="s">
+        <v>128</v>
       </c>
       <c r="D7">
         <v>343</v>
@@ -1606,8 +1618,8 @@
       <c r="B8" t="s">
         <v>42</v>
       </c>
-      <c r="C8">
-        <v>2020</v>
+      <c r="C8" t="s">
+        <v>129</v>
       </c>
       <c r="D8">
         <v>368</v>
@@ -1620,8 +1632,8 @@
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9">
-        <v>2021</v>
+      <c r="C9" t="s">
+        <v>130</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1634,8 +1646,8 @@
       <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="C10">
-        <v>2018</v>
+      <c r="C10" t="s">
+        <v>127</v>
       </c>
       <c r="D10">
         <v>684</v>
@@ -1648,8 +1660,8 @@
       <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C11">
-        <v>2019</v>
+      <c r="C11" t="s">
+        <v>128</v>
       </c>
       <c r="D11">
         <v>683</v>
@@ -1662,8 +1674,8 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12">
-        <v>2020</v>
+      <c r="C12" t="s">
+        <v>129</v>
       </c>
       <c r="D12">
         <v>678</v>
@@ -1676,8 +1688,8 @@
       <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="C13">
-        <v>2021</v>
+      <c r="C13" t="s">
+        <v>130</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1690,8 +1702,8 @@
       <c r="B14" t="s">
         <v>126</v>
       </c>
-      <c r="C14">
-        <v>2018</v>
+      <c r="C14" t="s">
+        <v>127</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1704,8 +1716,8 @@
       <c r="B15" t="s">
         <v>126</v>
       </c>
-      <c r="C15">
-        <v>2019</v>
+      <c r="C15" t="s">
+        <v>128</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1718,8 +1730,8 @@
       <c r="B16" t="s">
         <v>126</v>
       </c>
-      <c r="C16">
-        <v>2020</v>
+      <c r="C16" t="s">
+        <v>129</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1732,8 +1744,8 @@
       <c r="B17" t="s">
         <v>126</v>
       </c>
-      <c r="C17">
-        <v>2021</v>
+      <c r="C17" t="s">
+        <v>130</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1746,8 +1758,8 @@
       <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C18">
-        <v>2018</v>
+      <c r="C18" t="s">
+        <v>127</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -1760,8 +1772,8 @@
       <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19">
-        <v>2019</v>
+      <c r="C19" t="s">
+        <v>128</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1774,8 +1786,8 @@
       <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C20">
-        <v>2020</v>
+      <c r="C20" t="s">
+        <v>129</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1788,8 +1800,8 @@
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21">
-        <v>2021</v>
+      <c r="C21" t="s">
+        <v>130</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1802,8 +1814,8 @@
       <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C22">
-        <v>2018</v>
+      <c r="C22" t="s">
+        <v>127</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1816,8 +1828,8 @@
       <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C23">
-        <v>2019</v>
+      <c r="C23" t="s">
+        <v>128</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1830,8 +1842,8 @@
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C24">
-        <v>2020</v>
+      <c r="C24" t="s">
+        <v>129</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1844,8 +1856,8 @@
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25">
-        <v>2021</v>
+      <c r="C25" t="s">
+        <v>130</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1858,8 +1870,8 @@
       <c r="B26" t="s">
         <v>126</v>
       </c>
-      <c r="C26">
-        <v>2018</v>
+      <c r="C26" t="s">
+        <v>127</v>
       </c>
       <c r="D26">
         <v>175</v>
@@ -1872,8 +1884,8 @@
       <c r="B27" t="s">
         <v>126</v>
       </c>
-      <c r="C27">
-        <v>2019</v>
+      <c r="C27" t="s">
+        <v>128</v>
       </c>
       <c r="D27">
         <v>193</v>
@@ -1886,8 +1898,8 @@
       <c r="B28" t="s">
         <v>126</v>
       </c>
-      <c r="C28">
-        <v>2020</v>
+      <c r="C28" t="s">
+        <v>129</v>
       </c>
       <c r="D28">
         <v>176</v>
@@ -1900,8 +1912,8 @@
       <c r="B29" t="s">
         <v>126</v>
       </c>
-      <c r="C29">
-        <v>2021</v>
+      <c r="C29" t="s">
+        <v>130</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1914,8 +1926,8 @@
       <c r="B30" t="s">
         <v>42</v>
       </c>
-      <c r="C30">
-        <v>2018</v>
+      <c r="C30" t="s">
+        <v>127</v>
       </c>
       <c r="D30">
         <v>219</v>
@@ -1928,8 +1940,8 @@
       <c r="B31" t="s">
         <v>42</v>
       </c>
-      <c r="C31">
-        <v>2019</v>
+      <c r="C31" t="s">
+        <v>128</v>
       </c>
       <c r="D31">
         <v>218</v>
@@ -1942,8 +1954,8 @@
       <c r="B32" t="s">
         <v>42</v>
       </c>
-      <c r="C32">
-        <v>2020</v>
+      <c r="C32" t="s">
+        <v>129</v>
       </c>
       <c r="D32">
         <v>191</v>
@@ -1956,8 +1968,8 @@
       <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C33">
-        <v>2021</v>
+      <c r="C33" t="s">
+        <v>130</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1970,8 +1982,8 @@
       <c r="B34" t="s">
         <v>41</v>
       </c>
-      <c r="C34">
-        <v>2018</v>
+      <c r="C34" t="s">
+        <v>127</v>
       </c>
       <c r="D34">
         <v>394</v>
@@ -1984,8 +1996,8 @@
       <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="C35">
-        <v>2019</v>
+      <c r="C35" t="s">
+        <v>128</v>
       </c>
       <c r="D35">
         <v>411</v>
@@ -1998,8 +2010,8 @@
       <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="C36">
-        <v>2020</v>
+      <c r="C36" t="s">
+        <v>129</v>
       </c>
       <c r="D36">
         <v>367</v>
@@ -2012,8 +2024,8 @@
       <c r="B37" t="s">
         <v>41</v>
       </c>
-      <c r="C37">
-        <v>2021</v>
+      <c r="C37" t="s">
+        <v>130</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2026,8 +2038,8 @@
       <c r="B38" t="s">
         <v>126</v>
       </c>
-      <c r="C38">
-        <v>2018</v>
+      <c r="C38" t="s">
+        <v>127</v>
       </c>
       <c r="D38">
         <v>789</v>
@@ -2040,8 +2052,8 @@
       <c r="B39" t="s">
         <v>126</v>
       </c>
-      <c r="C39">
-        <v>2019</v>
+      <c r="C39" t="s">
+        <v>128</v>
       </c>
       <c r="D39">
         <v>770</v>
@@ -2054,8 +2066,8 @@
       <c r="B40" t="s">
         <v>126</v>
       </c>
-      <c r="C40">
-        <v>2020</v>
+      <c r="C40" t="s">
+        <v>129</v>
       </c>
       <c r="D40">
         <v>759</v>
@@ -2068,8 +2080,8 @@
       <c r="B41" t="s">
         <v>126</v>
       </c>
-      <c r="C41">
-        <v>2021</v>
+      <c r="C41" t="s">
+        <v>130</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2082,8 +2094,8 @@
       <c r="B42" t="s">
         <v>42</v>
       </c>
-      <c r="C42">
-        <v>2018</v>
+      <c r="C42" t="s">
+        <v>127</v>
       </c>
       <c r="D42">
         <v>1059</v>
@@ -2096,8 +2108,8 @@
       <c r="B43" t="s">
         <v>42</v>
       </c>
-      <c r="C43">
-        <v>2019</v>
+      <c r="C43" t="s">
+        <v>128</v>
       </c>
       <c r="D43">
         <v>996</v>
@@ -2110,8 +2122,8 @@
       <c r="B44" t="s">
         <v>42</v>
       </c>
-      <c r="C44">
-        <v>2020</v>
+      <c r="C44" t="s">
+        <v>129</v>
       </c>
       <c r="D44">
         <v>938</v>
@@ -2124,8 +2136,8 @@
       <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="C45">
-        <v>2021</v>
+      <c r="C45" t="s">
+        <v>130</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2138,8 +2150,8 @@
       <c r="B46" t="s">
         <v>41</v>
       </c>
-      <c r="C46">
-        <v>2018</v>
+      <c r="C46" t="s">
+        <v>127</v>
       </c>
       <c r="D46">
         <v>1848</v>
@@ -2152,8 +2164,8 @@
       <c r="B47" t="s">
         <v>41</v>
       </c>
-      <c r="C47">
-        <v>2019</v>
+      <c r="C47" t="s">
+        <v>128</v>
       </c>
       <c r="D47">
         <v>1766</v>
@@ -2166,8 +2178,8 @@
       <c r="B48" t="s">
         <v>41</v>
       </c>
-      <c r="C48">
-        <v>2020</v>
+      <c r="C48" t="s">
+        <v>129</v>
       </c>
       <c r="D48">
         <v>1697</v>
@@ -2180,8 +2192,8 @@
       <c r="B49" t="s">
         <v>41</v>
       </c>
-      <c r="C49">
-        <v>2021</v>
+      <c r="C49" t="s">
+        <v>130</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2194,8 +2206,8 @@
       <c r="B50" t="s">
         <v>126</v>
       </c>
-      <c r="C50">
-        <v>2018</v>
+      <c r="C50" t="s">
+        <v>127</v>
       </c>
       <c r="D50">
         <v>632</v>
@@ -2208,8 +2220,8 @@
       <c r="B51" t="s">
         <v>126</v>
       </c>
-      <c r="C51">
-        <v>2019</v>
+      <c r="C51" t="s">
+        <v>128</v>
       </c>
       <c r="D51">
         <v>542</v>
@@ -2222,8 +2234,8 @@
       <c r="B52" t="s">
         <v>126</v>
       </c>
-      <c r="C52">
-        <v>2020</v>
+      <c r="C52" t="s">
+        <v>129</v>
       </c>
       <c r="D52">
         <v>525</v>
@@ -2236,8 +2248,8 @@
       <c r="B53" t="s">
         <v>126</v>
       </c>
-      <c r="C53">
-        <v>2021</v>
+      <c r="C53" t="s">
+        <v>130</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2250,8 +2262,8 @@
       <c r="B54" t="s">
         <v>42</v>
       </c>
-      <c r="C54">
-        <v>2018</v>
+      <c r="C54" t="s">
+        <v>127</v>
       </c>
       <c r="D54">
         <v>692</v>
@@ -2264,8 +2276,8 @@
       <c r="B55" t="s">
         <v>42</v>
       </c>
-      <c r="C55">
-        <v>2019</v>
+      <c r="C55" t="s">
+        <v>128</v>
       </c>
       <c r="D55">
         <v>665</v>
@@ -2278,8 +2290,8 @@
       <c r="B56" t="s">
         <v>42</v>
       </c>
-      <c r="C56">
-        <v>2020</v>
+      <c r="C56" t="s">
+        <v>129</v>
       </c>
       <c r="D56">
         <v>684</v>
@@ -2292,8 +2304,8 @@
       <c r="B57" t="s">
         <v>42</v>
       </c>
-      <c r="C57">
-        <v>2021</v>
+      <c r="C57" t="s">
+        <v>130</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2306,8 +2318,8 @@
       <c r="B58" t="s">
         <v>41</v>
       </c>
-      <c r="C58">
-        <v>2018</v>
+      <c r="C58" t="s">
+        <v>127</v>
       </c>
       <c r="D58">
         <v>1324</v>
@@ -2320,8 +2332,8 @@
       <c r="B59" t="s">
         <v>41</v>
       </c>
-      <c r="C59">
-        <v>2019</v>
+      <c r="C59" t="s">
+        <v>128</v>
       </c>
       <c r="D59">
         <v>1207</v>
@@ -2334,8 +2346,8 @@
       <c r="B60" t="s">
         <v>41</v>
       </c>
-      <c r="C60">
-        <v>2020</v>
+      <c r="C60" t="s">
+        <v>129</v>
       </c>
       <c r="D60">
         <v>1209</v>
@@ -2348,8 +2360,8 @@
       <c r="B61" t="s">
         <v>41</v>
       </c>
-      <c r="C61">
-        <v>2021</v>
+      <c r="C61" t="s">
+        <v>130</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2362,8 +2374,8 @@
       <c r="B62" t="s">
         <v>126</v>
       </c>
-      <c r="C62">
-        <v>2018</v>
+      <c r="C62" t="s">
+        <v>127</v>
       </c>
       <c r="D62">
         <v>24461</v>
@@ -2376,8 +2388,8 @@
       <c r="B63" t="s">
         <v>126</v>
       </c>
-      <c r="C63">
-        <v>2019</v>
+      <c r="C63" t="s">
+        <v>128</v>
       </c>
       <c r="D63">
         <v>24782</v>
@@ -2390,8 +2402,8 @@
       <c r="B64" t="s">
         <v>126</v>
       </c>
-      <c r="C64">
-        <v>2020</v>
+      <c r="C64" t="s">
+        <v>129</v>
       </c>
       <c r="D64">
         <v>25157</v>
@@ -2404,8 +2416,8 @@
       <c r="B65" t="s">
         <v>126</v>
       </c>
-      <c r="C65">
-        <v>2021</v>
+      <c r="C65" t="s">
+        <v>130</v>
       </c>
       <c r="D65">
         <v>25525</v>
@@ -2418,8 +2430,8 @@
       <c r="B66" t="s">
         <v>42</v>
       </c>
-      <c r="C66">
-        <v>2018</v>
+      <c r="C66" t="s">
+        <v>127</v>
       </c>
       <c r="D66">
         <v>26003</v>
@@ -2432,8 +2444,8 @@
       <c r="B67" t="s">
         <v>42</v>
       </c>
-      <c r="C67">
-        <v>2019</v>
+      <c r="C67" t="s">
+        <v>128</v>
       </c>
       <c r="D67">
         <v>26496</v>
@@ -2446,8 +2458,8 @@
       <c r="B68" t="s">
         <v>42</v>
       </c>
-      <c r="C68">
-        <v>2020</v>
+      <c r="C68" t="s">
+        <v>129</v>
       </c>
       <c r="D68">
         <v>26952</v>
@@ -2460,8 +2472,8 @@
       <c r="B69" t="s">
         <v>42</v>
       </c>
-      <c r="C69">
-        <v>2021</v>
+      <c r="C69" t="s">
+        <v>130</v>
       </c>
       <c r="D69">
         <v>27384</v>
@@ -2474,8 +2486,8 @@
       <c r="B70" t="s">
         <v>41</v>
       </c>
-      <c r="C70">
-        <v>2018</v>
+      <c r="C70" t="s">
+        <v>127</v>
       </c>
       <c r="D70">
         <v>50464</v>
@@ -2488,8 +2500,8 @@
       <c r="B71" t="s">
         <v>41</v>
       </c>
-      <c r="C71">
-        <v>2019</v>
+      <c r="C71" t="s">
+        <v>128</v>
       </c>
       <c r="D71">
         <v>51278</v>
@@ -2502,8 +2514,8 @@
       <c r="B72" t="s">
         <v>41</v>
       </c>
-      <c r="C72">
-        <v>2020</v>
+      <c r="C72" t="s">
+        <v>129</v>
       </c>
       <c r="D72">
         <v>52109</v>
@@ -2516,8 +2528,8 @@
       <c r="B73" t="s">
         <v>41</v>
       </c>
-      <c r="C73">
-        <v>2021</v>
+      <c r="C73" t="s">
+        <v>130</v>
       </c>
       <c r="D73">
         <v>52909</v>
@@ -2530,8 +2542,8 @@
       <c r="B74" t="s">
         <v>126</v>
       </c>
-      <c r="C74">
-        <v>2018</v>
+      <c r="C74" t="s">
+        <v>127</v>
       </c>
       <c r="D74">
         <v>24782</v>
@@ -2544,8 +2556,8 @@
       <c r="B75" t="s">
         <v>126</v>
       </c>
-      <c r="C75">
-        <v>2019</v>
+      <c r="C75" t="s">
+        <v>128</v>
       </c>
       <c r="D75">
         <v>25157</v>
@@ -2558,8 +2570,8 @@
       <c r="B76" t="s">
         <v>126</v>
       </c>
-      <c r="C76">
-        <v>2020</v>
+      <c r="C76" t="s">
+        <v>129</v>
       </c>
       <c r="D76">
         <v>25525</v>
@@ -2572,8 +2584,8 @@
       <c r="B77" t="s">
         <v>126</v>
       </c>
-      <c r="C77">
-        <v>2021</v>
+      <c r="C77" t="s">
+        <v>130</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2586,8 +2598,8 @@
       <c r="B78" t="s">
         <v>42</v>
       </c>
-      <c r="C78">
-        <v>2018</v>
+      <c r="C78" t="s">
+        <v>127</v>
       </c>
       <c r="D78">
         <v>26496</v>
@@ -2600,8 +2612,8 @@
       <c r="B79" t="s">
         <v>42</v>
       </c>
-      <c r="C79">
-        <v>2019</v>
+      <c r="C79" t="s">
+        <v>128</v>
       </c>
       <c r="D79">
         <v>26952</v>
@@ -2614,8 +2626,8 @@
       <c r="B80" t="s">
         <v>42</v>
       </c>
-      <c r="C80">
-        <v>2020</v>
+      <c r="C80" t="s">
+        <v>129</v>
       </c>
       <c r="D80">
         <v>27384</v>
@@ -2628,8 +2640,8 @@
       <c r="B81" t="s">
         <v>42</v>
       </c>
-      <c r="C81">
-        <v>2021</v>
+      <c r="C81" t="s">
+        <v>130</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2642,8 +2654,8 @@
       <c r="B82" t="s">
         <v>41</v>
       </c>
-      <c r="C82">
-        <v>2018</v>
+      <c r="C82" t="s">
+        <v>127</v>
       </c>
       <c r="D82">
         <v>51278</v>
@@ -2656,8 +2668,8 @@
       <c r="B83" t="s">
         <v>41</v>
       </c>
-      <c r="C83">
-        <v>2019</v>
+      <c r="C83" t="s">
+        <v>128</v>
       </c>
       <c r="D83">
         <v>52109</v>
@@ -2670,8 +2682,8 @@
       <c r="B84" t="s">
         <v>41</v>
       </c>
-      <c r="C84">
-        <v>2020</v>
+      <c r="C84" t="s">
+        <v>129</v>
       </c>
       <c r="D84">
         <v>52909</v>
@@ -2684,8 +2696,8 @@
       <c r="B85" t="s">
         <v>41</v>
       </c>
-      <c r="C85">
-        <v>2021</v>
+      <c r="C85" t="s">
+        <v>130</v>
       </c>
       <c r="D85">
         <v>0</v>

</xml_diff>

<commit_message>
Add support for timevals (#83)
Close  #39
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6096C0ED-2C6B-4E07-95F1-A08343F99294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699A3483-62AD-4871-95E2-5634DBD21323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="615" windowWidth="16995" windowHeight="31785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21510" yWindow="4215" windowWidth="23730" windowHeight="20625" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="131">
   <si>
     <t>type</t>
   </si>
@@ -404,6 +404,18 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>2000Q1</t>
+  </si>
+  <si>
+    <t>2000Q2</t>
+  </si>
+  <si>
+    <t>2000Q3</t>
+  </si>
+  <si>
+    <t>2000Q4</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1495,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1522,8 +1534,8 @@
       <c r="B2" t="s">
         <v>126</v>
       </c>
-      <c r="C2">
-        <v>2018</v>
+      <c r="C2" t="s">
+        <v>127</v>
       </c>
       <c r="D2">
         <v>338</v>
@@ -1536,8 +1548,8 @@
       <c r="B3" t="s">
         <v>126</v>
       </c>
-      <c r="C3">
-        <v>2019</v>
+      <c r="C3" t="s">
+        <v>128</v>
       </c>
       <c r="D3">
         <v>340</v>
@@ -1550,8 +1562,8 @@
       <c r="B4" t="s">
         <v>126</v>
       </c>
-      <c r="C4">
-        <v>2020</v>
+      <c r="C4" t="s">
+        <v>129</v>
       </c>
       <c r="D4">
         <v>310</v>
@@ -1564,8 +1576,8 @@
       <c r="B5" t="s">
         <v>126</v>
       </c>
-      <c r="C5">
-        <v>2021</v>
+      <c r="C5" t="s">
+        <v>130</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1578,8 +1590,8 @@
       <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C6">
-        <v>2018</v>
+      <c r="C6" t="s">
+        <v>127</v>
       </c>
       <c r="D6">
         <v>346</v>
@@ -1592,8 +1604,8 @@
       <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7">
-        <v>2019</v>
+      <c r="C7" t="s">
+        <v>128</v>
       </c>
       <c r="D7">
         <v>343</v>
@@ -1606,8 +1618,8 @@
       <c r="B8" t="s">
         <v>42</v>
       </c>
-      <c r="C8">
-        <v>2020</v>
+      <c r="C8" t="s">
+        <v>129</v>
       </c>
       <c r="D8">
         <v>368</v>
@@ -1620,8 +1632,8 @@
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9">
-        <v>2021</v>
+      <c r="C9" t="s">
+        <v>130</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1634,8 +1646,8 @@
       <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="C10">
-        <v>2018</v>
+      <c r="C10" t="s">
+        <v>127</v>
       </c>
       <c r="D10">
         <v>684</v>
@@ -1648,8 +1660,8 @@
       <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C11">
-        <v>2019</v>
+      <c r="C11" t="s">
+        <v>128</v>
       </c>
       <c r="D11">
         <v>683</v>
@@ -1662,8 +1674,8 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12">
-        <v>2020</v>
+      <c r="C12" t="s">
+        <v>129</v>
       </c>
       <c r="D12">
         <v>678</v>
@@ -1676,8 +1688,8 @@
       <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="C13">
-        <v>2021</v>
+      <c r="C13" t="s">
+        <v>130</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1690,8 +1702,8 @@
       <c r="B14" t="s">
         <v>126</v>
       </c>
-      <c r="C14">
-        <v>2018</v>
+      <c r="C14" t="s">
+        <v>127</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1704,8 +1716,8 @@
       <c r="B15" t="s">
         <v>126</v>
       </c>
-      <c r="C15">
-        <v>2019</v>
+      <c r="C15" t="s">
+        <v>128</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1718,8 +1730,8 @@
       <c r="B16" t="s">
         <v>126</v>
       </c>
-      <c r="C16">
-        <v>2020</v>
+      <c r="C16" t="s">
+        <v>129</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1732,8 +1744,8 @@
       <c r="B17" t="s">
         <v>126</v>
       </c>
-      <c r="C17">
-        <v>2021</v>
+      <c r="C17" t="s">
+        <v>130</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1746,8 +1758,8 @@
       <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C18">
-        <v>2018</v>
+      <c r="C18" t="s">
+        <v>127</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -1760,8 +1772,8 @@
       <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19">
-        <v>2019</v>
+      <c r="C19" t="s">
+        <v>128</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1774,8 +1786,8 @@
       <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C20">
-        <v>2020</v>
+      <c r="C20" t="s">
+        <v>129</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1788,8 +1800,8 @@
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21">
-        <v>2021</v>
+      <c r="C21" t="s">
+        <v>130</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1802,8 +1814,8 @@
       <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C22">
-        <v>2018</v>
+      <c r="C22" t="s">
+        <v>127</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1816,8 +1828,8 @@
       <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C23">
-        <v>2019</v>
+      <c r="C23" t="s">
+        <v>128</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1830,8 +1842,8 @@
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C24">
-        <v>2020</v>
+      <c r="C24" t="s">
+        <v>129</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1844,8 +1856,8 @@
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25">
-        <v>2021</v>
+      <c r="C25" t="s">
+        <v>130</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1858,8 +1870,8 @@
       <c r="B26" t="s">
         <v>126</v>
       </c>
-      <c r="C26">
-        <v>2018</v>
+      <c r="C26" t="s">
+        <v>127</v>
       </c>
       <c r="D26">
         <v>175</v>
@@ -1872,8 +1884,8 @@
       <c r="B27" t="s">
         <v>126</v>
       </c>
-      <c r="C27">
-        <v>2019</v>
+      <c r="C27" t="s">
+        <v>128</v>
       </c>
       <c r="D27">
         <v>193</v>
@@ -1886,8 +1898,8 @@
       <c r="B28" t="s">
         <v>126</v>
       </c>
-      <c r="C28">
-        <v>2020</v>
+      <c r="C28" t="s">
+        <v>129</v>
       </c>
       <c r="D28">
         <v>176</v>
@@ -1900,8 +1912,8 @@
       <c r="B29" t="s">
         <v>126</v>
       </c>
-      <c r="C29">
-        <v>2021</v>
+      <c r="C29" t="s">
+        <v>130</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1914,8 +1926,8 @@
       <c r="B30" t="s">
         <v>42</v>
       </c>
-      <c r="C30">
-        <v>2018</v>
+      <c r="C30" t="s">
+        <v>127</v>
       </c>
       <c r="D30">
         <v>219</v>
@@ -1928,8 +1940,8 @@
       <c r="B31" t="s">
         <v>42</v>
       </c>
-      <c r="C31">
-        <v>2019</v>
+      <c r="C31" t="s">
+        <v>128</v>
       </c>
       <c r="D31">
         <v>218</v>
@@ -1942,8 +1954,8 @@
       <c r="B32" t="s">
         <v>42</v>
       </c>
-      <c r="C32">
-        <v>2020</v>
+      <c r="C32" t="s">
+        <v>129</v>
       </c>
       <c r="D32">
         <v>191</v>
@@ -1956,8 +1968,8 @@
       <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C33">
-        <v>2021</v>
+      <c r="C33" t="s">
+        <v>130</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1970,8 +1982,8 @@
       <c r="B34" t="s">
         <v>41</v>
       </c>
-      <c r="C34">
-        <v>2018</v>
+      <c r="C34" t="s">
+        <v>127</v>
       </c>
       <c r="D34">
         <v>394</v>
@@ -1984,8 +1996,8 @@
       <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="C35">
-        <v>2019</v>
+      <c r="C35" t="s">
+        <v>128</v>
       </c>
       <c r="D35">
         <v>411</v>
@@ -1998,8 +2010,8 @@
       <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="C36">
-        <v>2020</v>
+      <c r="C36" t="s">
+        <v>129</v>
       </c>
       <c r="D36">
         <v>367</v>
@@ -2012,8 +2024,8 @@
       <c r="B37" t="s">
         <v>41</v>
       </c>
-      <c r="C37">
-        <v>2021</v>
+      <c r="C37" t="s">
+        <v>130</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2026,8 +2038,8 @@
       <c r="B38" t="s">
         <v>126</v>
       </c>
-      <c r="C38">
-        <v>2018</v>
+      <c r="C38" t="s">
+        <v>127</v>
       </c>
       <c r="D38">
         <v>789</v>
@@ -2040,8 +2052,8 @@
       <c r="B39" t="s">
         <v>126</v>
       </c>
-      <c r="C39">
-        <v>2019</v>
+      <c r="C39" t="s">
+        <v>128</v>
       </c>
       <c r="D39">
         <v>770</v>
@@ -2054,8 +2066,8 @@
       <c r="B40" t="s">
         <v>126</v>
       </c>
-      <c r="C40">
-        <v>2020</v>
+      <c r="C40" t="s">
+        <v>129</v>
       </c>
       <c r="D40">
         <v>759</v>
@@ -2068,8 +2080,8 @@
       <c r="B41" t="s">
         <v>126</v>
       </c>
-      <c r="C41">
-        <v>2021</v>
+      <c r="C41" t="s">
+        <v>130</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2082,8 +2094,8 @@
       <c r="B42" t="s">
         <v>42</v>
       </c>
-      <c r="C42">
-        <v>2018</v>
+      <c r="C42" t="s">
+        <v>127</v>
       </c>
       <c r="D42">
         <v>1059</v>
@@ -2096,8 +2108,8 @@
       <c r="B43" t="s">
         <v>42</v>
       </c>
-      <c r="C43">
-        <v>2019</v>
+      <c r="C43" t="s">
+        <v>128</v>
       </c>
       <c r="D43">
         <v>996</v>
@@ -2110,8 +2122,8 @@
       <c r="B44" t="s">
         <v>42</v>
       </c>
-      <c r="C44">
-        <v>2020</v>
+      <c r="C44" t="s">
+        <v>129</v>
       </c>
       <c r="D44">
         <v>938</v>
@@ -2124,8 +2136,8 @@
       <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="C45">
-        <v>2021</v>
+      <c r="C45" t="s">
+        <v>130</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2138,8 +2150,8 @@
       <c r="B46" t="s">
         <v>41</v>
       </c>
-      <c r="C46">
-        <v>2018</v>
+      <c r="C46" t="s">
+        <v>127</v>
       </c>
       <c r="D46">
         <v>1848</v>
@@ -2152,8 +2164,8 @@
       <c r="B47" t="s">
         <v>41</v>
       </c>
-      <c r="C47">
-        <v>2019</v>
+      <c r="C47" t="s">
+        <v>128</v>
       </c>
       <c r="D47">
         <v>1766</v>
@@ -2166,8 +2178,8 @@
       <c r="B48" t="s">
         <v>41</v>
       </c>
-      <c r="C48">
-        <v>2020</v>
+      <c r="C48" t="s">
+        <v>129</v>
       </c>
       <c r="D48">
         <v>1697</v>
@@ -2180,8 +2192,8 @@
       <c r="B49" t="s">
         <v>41</v>
       </c>
-      <c r="C49">
-        <v>2021</v>
+      <c r="C49" t="s">
+        <v>130</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2194,8 +2206,8 @@
       <c r="B50" t="s">
         <v>126</v>
       </c>
-      <c r="C50">
-        <v>2018</v>
+      <c r="C50" t="s">
+        <v>127</v>
       </c>
       <c r="D50">
         <v>632</v>
@@ -2208,8 +2220,8 @@
       <c r="B51" t="s">
         <v>126</v>
       </c>
-      <c r="C51">
-        <v>2019</v>
+      <c r="C51" t="s">
+        <v>128</v>
       </c>
       <c r="D51">
         <v>542</v>
@@ -2222,8 +2234,8 @@
       <c r="B52" t="s">
         <v>126</v>
       </c>
-      <c r="C52">
-        <v>2020</v>
+      <c r="C52" t="s">
+        <v>129</v>
       </c>
       <c r="D52">
         <v>525</v>
@@ -2236,8 +2248,8 @@
       <c r="B53" t="s">
         <v>126</v>
       </c>
-      <c r="C53">
-        <v>2021</v>
+      <c r="C53" t="s">
+        <v>130</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2250,8 +2262,8 @@
       <c r="B54" t="s">
         <v>42</v>
       </c>
-      <c r="C54">
-        <v>2018</v>
+      <c r="C54" t="s">
+        <v>127</v>
       </c>
       <c r="D54">
         <v>692</v>
@@ -2264,8 +2276,8 @@
       <c r="B55" t="s">
         <v>42</v>
       </c>
-      <c r="C55">
-        <v>2019</v>
+      <c r="C55" t="s">
+        <v>128</v>
       </c>
       <c r="D55">
         <v>665</v>
@@ -2278,8 +2290,8 @@
       <c r="B56" t="s">
         <v>42</v>
       </c>
-      <c r="C56">
-        <v>2020</v>
+      <c r="C56" t="s">
+        <v>129</v>
       </c>
       <c r="D56">
         <v>684</v>
@@ -2292,8 +2304,8 @@
       <c r="B57" t="s">
         <v>42</v>
       </c>
-      <c r="C57">
-        <v>2021</v>
+      <c r="C57" t="s">
+        <v>130</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2306,8 +2318,8 @@
       <c r="B58" t="s">
         <v>41</v>
       </c>
-      <c r="C58">
-        <v>2018</v>
+      <c r="C58" t="s">
+        <v>127</v>
       </c>
       <c r="D58">
         <v>1324</v>
@@ -2320,8 +2332,8 @@
       <c r="B59" t="s">
         <v>41</v>
       </c>
-      <c r="C59">
-        <v>2019</v>
+      <c r="C59" t="s">
+        <v>128</v>
       </c>
       <c r="D59">
         <v>1207</v>
@@ -2334,8 +2346,8 @@
       <c r="B60" t="s">
         <v>41</v>
       </c>
-      <c r="C60">
-        <v>2020</v>
+      <c r="C60" t="s">
+        <v>129</v>
       </c>
       <c r="D60">
         <v>1209</v>
@@ -2348,8 +2360,8 @@
       <c r="B61" t="s">
         <v>41</v>
       </c>
-      <c r="C61">
-        <v>2021</v>
+      <c r="C61" t="s">
+        <v>130</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2362,8 +2374,8 @@
       <c r="B62" t="s">
         <v>126</v>
       </c>
-      <c r="C62">
-        <v>2018</v>
+      <c r="C62" t="s">
+        <v>127</v>
       </c>
       <c r="D62">
         <v>24461</v>
@@ -2376,8 +2388,8 @@
       <c r="B63" t="s">
         <v>126</v>
       </c>
-      <c r="C63">
-        <v>2019</v>
+      <c r="C63" t="s">
+        <v>128</v>
       </c>
       <c r="D63">
         <v>24782</v>
@@ -2390,8 +2402,8 @@
       <c r="B64" t="s">
         <v>126</v>
       </c>
-      <c r="C64">
-        <v>2020</v>
+      <c r="C64" t="s">
+        <v>129</v>
       </c>
       <c r="D64">
         <v>25157</v>
@@ -2404,8 +2416,8 @@
       <c r="B65" t="s">
         <v>126</v>
       </c>
-      <c r="C65">
-        <v>2021</v>
+      <c r="C65" t="s">
+        <v>130</v>
       </c>
       <c r="D65">
         <v>25525</v>
@@ -2418,8 +2430,8 @@
       <c r="B66" t="s">
         <v>42</v>
       </c>
-      <c r="C66">
-        <v>2018</v>
+      <c r="C66" t="s">
+        <v>127</v>
       </c>
       <c r="D66">
         <v>26003</v>
@@ -2432,8 +2444,8 @@
       <c r="B67" t="s">
         <v>42</v>
       </c>
-      <c r="C67">
-        <v>2019</v>
+      <c r="C67" t="s">
+        <v>128</v>
       </c>
       <c r="D67">
         <v>26496</v>
@@ -2446,8 +2458,8 @@
       <c r="B68" t="s">
         <v>42</v>
       </c>
-      <c r="C68">
-        <v>2020</v>
+      <c r="C68" t="s">
+        <v>129</v>
       </c>
       <c r="D68">
         <v>26952</v>
@@ -2460,8 +2472,8 @@
       <c r="B69" t="s">
         <v>42</v>
       </c>
-      <c r="C69">
-        <v>2021</v>
+      <c r="C69" t="s">
+        <v>130</v>
       </c>
       <c r="D69">
         <v>27384</v>
@@ -2474,8 +2486,8 @@
       <c r="B70" t="s">
         <v>41</v>
       </c>
-      <c r="C70">
-        <v>2018</v>
+      <c r="C70" t="s">
+        <v>127</v>
       </c>
       <c r="D70">
         <v>50464</v>
@@ -2488,8 +2500,8 @@
       <c r="B71" t="s">
         <v>41</v>
       </c>
-      <c r="C71">
-        <v>2019</v>
+      <c r="C71" t="s">
+        <v>128</v>
       </c>
       <c r="D71">
         <v>51278</v>
@@ -2502,8 +2514,8 @@
       <c r="B72" t="s">
         <v>41</v>
       </c>
-      <c r="C72">
-        <v>2020</v>
+      <c r="C72" t="s">
+        <v>129</v>
       </c>
       <c r="D72">
         <v>52109</v>
@@ -2516,8 +2528,8 @@
       <c r="B73" t="s">
         <v>41</v>
       </c>
-      <c r="C73">
-        <v>2021</v>
+      <c r="C73" t="s">
+        <v>130</v>
       </c>
       <c r="D73">
         <v>52909</v>
@@ -2530,8 +2542,8 @@
       <c r="B74" t="s">
         <v>126</v>
       </c>
-      <c r="C74">
-        <v>2018</v>
+      <c r="C74" t="s">
+        <v>127</v>
       </c>
       <c r="D74">
         <v>24782</v>
@@ -2544,8 +2556,8 @@
       <c r="B75" t="s">
         <v>126</v>
       </c>
-      <c r="C75">
-        <v>2019</v>
+      <c r="C75" t="s">
+        <v>128</v>
       </c>
       <c r="D75">
         <v>25157</v>
@@ -2558,8 +2570,8 @@
       <c r="B76" t="s">
         <v>126</v>
       </c>
-      <c r="C76">
-        <v>2020</v>
+      <c r="C76" t="s">
+        <v>129</v>
       </c>
       <c r="D76">
         <v>25525</v>
@@ -2572,8 +2584,8 @@
       <c r="B77" t="s">
         <v>126</v>
       </c>
-      <c r="C77">
-        <v>2021</v>
+      <c r="C77" t="s">
+        <v>130</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2586,8 +2598,8 @@
       <c r="B78" t="s">
         <v>42</v>
       </c>
-      <c r="C78">
-        <v>2018</v>
+      <c r="C78" t="s">
+        <v>127</v>
       </c>
       <c r="D78">
         <v>26496</v>
@@ -2600,8 +2612,8 @@
       <c r="B79" t="s">
         <v>42</v>
       </c>
-      <c r="C79">
-        <v>2019</v>
+      <c r="C79" t="s">
+        <v>128</v>
       </c>
       <c r="D79">
         <v>26952</v>
@@ -2614,8 +2626,8 @@
       <c r="B80" t="s">
         <v>42</v>
       </c>
-      <c r="C80">
-        <v>2020</v>
+      <c r="C80" t="s">
+        <v>129</v>
       </c>
       <c r="D80">
         <v>27384</v>
@@ -2628,8 +2640,8 @@
       <c r="B81" t="s">
         <v>42</v>
       </c>
-      <c r="C81">
-        <v>2021</v>
+      <c r="C81" t="s">
+        <v>130</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2642,8 +2654,8 @@
       <c r="B82" t="s">
         <v>41</v>
       </c>
-      <c r="C82">
-        <v>2018</v>
+      <c r="C82" t="s">
+        <v>127</v>
       </c>
       <c r="D82">
         <v>51278</v>
@@ -2656,8 +2668,8 @@
       <c r="B83" t="s">
         <v>41</v>
       </c>
-      <c r="C83">
-        <v>2019</v>
+      <c r="C83" t="s">
+        <v>128</v>
       </c>
       <c r="D83">
         <v>52109</v>
@@ -2670,8 +2682,8 @@
       <c r="B84" t="s">
         <v>41</v>
       </c>
-      <c r="C84">
-        <v>2020</v>
+      <c r="C84" t="s">
+        <v>129</v>
       </c>
       <c r="D84">
         <v>52909</v>
@@ -2684,8 +2696,8 @@
       <c r="B85" t="s">
         <v>41</v>
       </c>
-      <c r="C85">
-        <v>2021</v>
+      <c r="C85" t="s">
+        <v>130</v>
       </c>
       <c r="D85">
         <v>0</v>

</xml_diff>

<commit_message>
Allow figures varaible to have any name
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699A3483-62AD-4871-95E2-5634DBD21323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5808D450-F47F-4DB9-9FE5-537344C86CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21510" yWindow="4215" windowWidth="23730" windowHeight="20625" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="31680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="132">
   <si>
     <t>type</t>
   </si>
@@ -416,13 +416,16 @@
   </si>
   <si>
     <t>2000Q4</t>
+  </si>
+  <si>
+    <t>figures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -450,6 +453,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -473,7 +481,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -482,6 +490,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1104,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1158,8 +1167,8 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1287,6 +1296,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1507,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1524,7 +1534,7 @@
         <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Create Excel metadata from px-file (#82)
Close  #39, close #87, close #84, close #73, close #91, close #68
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699A3483-62AD-4871-95E2-5634DBD21323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5808D450-F47F-4DB9-9FE5-537344C86CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21510" yWindow="4215" windowWidth="23730" windowHeight="20625" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="31680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="132">
   <si>
     <t>type</t>
   </si>
@@ -416,13 +416,16 @@
   </si>
   <si>
     <t>2000Q4</t>
+  </si>
+  <si>
+    <t>figures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -450,6 +453,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -473,7 +481,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -482,6 +490,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1104,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1158,8 +1167,8 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1287,6 +1296,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1507,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1524,7 +1534,7 @@
         <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Support other main language than English
Close #54
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\My Drive\new\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2F76B1-DF00-44CE-A6B3-A09247339CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B311EBB1-27E0-434E-B8A6-88E10E48B35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="0" windowWidth="32850" windowHeight="31680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -23,20 +23,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="99">
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>en_note</t>
-  </si>
-  <si>
-    <t>en_elimination</t>
-  </si>
-  <si>
-    <t>en_domain</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -58,57 +49,21 @@
     <t>value</t>
   </si>
   <si>
-    <t>CONTACT_en</t>
-  </si>
-  <si>
-    <t>NOTE_en</t>
-  </si>
-  <si>
-    <t>CONTENTS_en</t>
-  </si>
-  <si>
-    <t>UNITS_en</t>
-  </si>
-  <si>
     <t>Grønlands Statistik</t>
   </si>
   <si>
-    <t>SOURCE_en</t>
-  </si>
-  <si>
-    <t>Statistics Greenland</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_en</t>
-  </si>
-  <si>
-    <t>LINK_en</t>
-  </si>
-  <si>
-    <t>Lars Pedersen, LARP@stat.gl</t>
-  </si>
-  <si>
     <t>Befolkningen 1. januar</t>
   </si>
   <si>
-    <t>Population January 1st</t>
-  </si>
-  <si>
     <t>personer</t>
   </si>
   <si>
-    <t>persons</t>
-  </si>
-  <si>
     <t>BE</t>
   </si>
   <si>
     <t>Befolkning</t>
   </si>
   <si>
-    <t>Population</t>
-  </si>
-  <si>
     <t>20190124 09:00</t>
   </si>
   <si>
@@ -118,9 +73,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
     <t>køn</t>
   </si>
   <si>
@@ -130,18 +82,9 @@
     <t>FIGURES</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>I alt</t>
   </si>
   <si>
-    <t>Men</t>
-  </si>
-  <si>
-    <t>Women</t>
-  </si>
-  <si>
     <t>Mænd</t>
   </si>
   <si>
@@ -175,15 +118,9 @@
     <t>www.stat.gl/bed202201/m1</t>
   </si>
   <si>
-    <t>www.stat.gl/bee202201/m1</t>
-  </si>
-  <si>
     <t>precision</t>
   </si>
   <si>
-    <t>TESTPopulation January 1st 2018-2022</t>
-  </si>
-  <si>
     <t>TESTBefolkningen pr 1. januar 2018 - 2022</t>
   </si>
   <si>
@@ -211,18 +148,12 @@
     <t>MATRIX</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
     <t>DECIMALS</t>
   </si>
   <si>
     <t>SHOWDECIMALS</t>
   </si>
   <si>
-    <t>NOTEX_en</t>
-  </si>
-  <si>
     <t>Tvungen fodnote</t>
   </si>
   <si>
@@ -238,9 +169,6 @@
     <t>ANSI</t>
   </si>
   <si>
-    <t>en","fo</t>
-  </si>
-  <si>
     <t>CONTACT_fo</t>
   </si>
   <si>
@@ -301,27 +229,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Population (start of year)</t>
-  </si>
-  <si>
-    <t>Birth</t>
-  </si>
-  <si>
-    <t>Immigration</t>
-  </si>
-  <si>
-    <t>Emigration</t>
-  </si>
-  <si>
-    <t>Death</t>
-  </si>
-  <si>
-    <t>Correction</t>
-  </si>
-  <si>
-    <t>Population (end of year)</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -385,24 +292,15 @@
     <t>SUBJECT-AREA_fo</t>
   </si>
   <si>
-    <t>SUBJECT-AREA_en</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
     <t>fo_long_name</t>
   </si>
   <si>
-    <t>en_long_name</t>
-  </si>
-  <si>
     <t>fo_code_label</t>
   </si>
   <si>
-    <t>en_code_label</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -419,6 +317,9 @@
   </si>
   <si>
     <t>figures</t>
+  </si>
+  <si>
+    <t>fo</t>
   </si>
 </sst>
 </file>
@@ -481,13 +382,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -831,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -844,152 +744,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>10</v>
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="4">
+        <v>82</v>
+      </c>
+      <c r="B3" s="3">
         <v>2000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
         <v>72</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -997,124 +897,51 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B30" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="B31" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K83" sqref="K83"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1122,177 +949,117 @@
     <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1">
-      <c r="A1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="5" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="B2" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="D15" s="3"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1302,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1314,197 +1081,163 @@
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1">
-      <c r="A1" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:5" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>126</v>
+      <c r="C11" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1517,35 +1250,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>131</v>
+      <c r="A1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D2">
         <v>338</v>
@@ -1553,13 +1286,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D3">
         <v>340</v>
@@ -1567,13 +1300,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D4">
         <v>310</v>
@@ -1581,13 +1314,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1595,13 +1328,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D6">
         <v>346</v>
@@ -1609,13 +1342,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D7">
         <v>343</v>
@@ -1623,13 +1356,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D8">
         <v>368</v>
@@ -1637,13 +1370,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1651,13 +1384,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D10">
         <v>684</v>
@@ -1665,13 +1398,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D11">
         <v>683</v>
@@ -1679,13 +1412,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D12">
         <v>678</v>
@@ -1693,13 +1426,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1707,13 +1440,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1721,13 +1454,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1735,13 +1468,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1749,13 +1482,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1763,13 +1496,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -1777,13 +1510,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1791,13 +1524,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1805,13 +1538,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1819,13 +1552,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1833,13 +1566,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1847,13 +1580,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1861,13 +1594,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1875,13 +1608,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D26">
         <v>175</v>
@@ -1889,13 +1622,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D27">
         <v>193</v>
@@ -1903,13 +1636,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D28">
         <v>176</v>
@@ -1917,13 +1650,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1931,13 +1664,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D30">
         <v>219</v>
@@ -1945,13 +1678,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D31">
         <v>218</v>
@@ -1959,13 +1692,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D32">
         <v>191</v>
@@ -1973,13 +1706,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1987,13 +1720,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D34">
         <v>394</v>
@@ -2001,13 +1734,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D35">
         <v>411</v>
@@ -2015,13 +1748,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D36">
         <v>367</v>
@@ -2029,13 +1762,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2043,13 +1776,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D38">
         <v>789</v>
@@ -2057,13 +1790,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D39">
         <v>770</v>
@@ -2071,13 +1804,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D40">
         <v>759</v>
@@ -2085,13 +1818,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2099,13 +1832,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D42">
         <v>1059</v>
@@ -2113,13 +1846,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D43">
         <v>996</v>
@@ -2127,13 +1860,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D44">
         <v>938</v>
@@ -2141,13 +1874,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2155,13 +1888,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D46">
         <v>1848</v>
@@ -2169,13 +1902,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D47">
         <v>1766</v>
@@ -2183,13 +1916,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D48">
         <v>1697</v>
@@ -2197,13 +1930,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2211,13 +1944,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D50">
         <v>632</v>
@@ -2225,13 +1958,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D51">
         <v>542</v>
@@ -2239,13 +1972,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D52">
         <v>525</v>
@@ -2253,13 +1986,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2267,13 +2000,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C54" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D54">
         <v>692</v>
@@ -2281,13 +2014,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C55" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D55">
         <v>665</v>
@@ -2295,13 +2028,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C56" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D56">
         <v>684</v>
@@ -2309,13 +2042,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2323,13 +2056,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D58">
         <v>1324</v>
@@ -2337,13 +2070,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D59">
         <v>1207</v>
@@ -2351,13 +2084,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D60">
         <v>1209</v>
@@ -2365,13 +2098,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2379,13 +2112,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D62">
         <v>24461</v>
@@ -2393,13 +2126,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C63" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D63">
         <v>24782</v>
@@ -2407,13 +2140,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C64" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D64">
         <v>25157</v>
@@ -2421,13 +2154,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C65" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D65">
         <v>25525</v>
@@ -2435,13 +2168,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C66" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D66">
         <v>26003</v>
@@ -2449,13 +2182,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D67">
         <v>26496</v>
@@ -2463,13 +2196,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D68">
         <v>26952</v>
@@ -2477,13 +2210,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C69" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D69">
         <v>27384</v>
@@ -2491,13 +2224,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C70" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D70">
         <v>50464</v>
@@ -2505,13 +2238,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D71">
         <v>51278</v>
@@ -2519,13 +2252,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D72">
         <v>52109</v>
@@ -2533,13 +2266,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C73" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D73">
         <v>52909</v>
@@ -2547,13 +2280,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B74" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C74" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D74">
         <v>24782</v>
@@ -2561,13 +2294,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C75" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D75">
         <v>25157</v>
@@ -2575,13 +2308,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C76" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D76">
         <v>25525</v>
@@ -2589,13 +2322,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C77" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2603,13 +2336,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C78" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D78">
         <v>26496</v>
@@ -2617,13 +2350,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B79" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D79">
         <v>26952</v>
@@ -2631,13 +2364,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D80">
         <v>27384</v>
@@ -2645,13 +2378,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B81" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C81" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2659,13 +2392,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B82" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C82" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D82">
         <v>51278</v>
@@ -2673,13 +2406,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B83" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C83" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D83">
         <v>52109</v>
@@ -2687,13 +2420,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B84" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D84">
         <v>52909</v>
@@ -2701,13 +2434,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D85">
         <v>0</v>

</xml_diff>

<commit_message>
Remove VARIABLECODE for figures variables
Close #133
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\My Drive\new\repo\pxmake\tests\testthat\fixtures\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B311EBB1-27E0-434E-B8A6-88E10E48B35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DE1AFA-A88F-4D3E-8A77-AB31AE9FB3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="32850" windowHeight="31680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31335" yWindow="9705" windowWidth="24210" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -316,10 +316,10 @@
     <t>2000Q4</t>
   </si>
   <si>
-    <t>figures</t>
-  </si>
-  <si>
     <t>fo</t>
+  </si>
+  <si>
+    <t>figures_</t>
   </si>
 </sst>
 </file>
@@ -772,7 +772,7 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -780,7 +780,7 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -980,7 +980,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1250,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -1267,7 +1267,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Bugfix: Support px-files without LANGUAGES keyword
Close #143
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DE1AFA-A88F-4D3E-8A77-AB31AE9FB3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AB6162-17F0-44B3-972B-0CBAAADE3109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31335" yWindow="9705" windowWidth="24210" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17475" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="98">
   <si>
     <t>type</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>LANGUAGE</t>
-  </si>
-  <si>
-    <t>LANGUAGES</t>
   </si>
   <si>
     <t>MATRIX</t>
@@ -731,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,12 +753,12 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="3">
         <v>2000</v>
@@ -772,7 +769,7 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -780,39 +777,39 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1">
       <c r="A8" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -820,7 +817,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -828,39 +825,39 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -868,7 +865,7 @@
         <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -876,7 +873,7 @@
         <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -884,15 +881,15 @@
         <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -905,31 +902,23 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
@@ -940,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -960,27 +949,27 @@
         <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1003,19 +992,19 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1023,7 +1012,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -1085,7 +1074,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -1094,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>31</v>
@@ -1102,105 +1091,105 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -1214,7 +1203,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -1228,13 +1217,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
@@ -1258,27 +1247,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>93</v>
       </c>
       <c r="D2">
         <v>338</v>
@@ -1286,13 +1275,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3">
         <v>340</v>
@@ -1300,13 +1289,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4">
         <v>310</v>
@@ -1314,13 +1303,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1328,13 +1317,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6">
         <v>346</v>
@@ -1342,13 +1331,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7">
         <v>343</v>
@@ -1356,13 +1345,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8">
         <v>368</v>
@@ -1370,13 +1359,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1384,13 +1373,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10">
         <v>684</v>
@@ -1398,13 +1387,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11">
         <v>683</v>
@@ -1412,13 +1401,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12">
         <v>678</v>
@@ -1426,13 +1415,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1440,13 +1429,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="s">
         <v>92</v>
-      </c>
-      <c r="C14" t="s">
-        <v>93</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1454,13 +1443,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1468,13 +1457,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1482,13 +1471,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1496,13 +1485,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -1510,13 +1499,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1524,13 +1513,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1538,13 +1527,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1552,13 +1541,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1566,13 +1555,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1580,13 +1569,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1594,13 +1583,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1608,13 +1597,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
         <v>92</v>
-      </c>
-      <c r="C26" t="s">
-        <v>93</v>
       </c>
       <c r="D26">
         <v>175</v>
@@ -1622,13 +1611,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D27">
         <v>193</v>
@@ -1636,13 +1625,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D28">
         <v>176</v>
@@ -1650,13 +1639,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1664,13 +1653,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D30">
         <v>219</v>
@@ -1678,13 +1667,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D31">
         <v>218</v>
@@ -1692,13 +1681,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D32">
         <v>191</v>
@@ -1706,13 +1695,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1720,13 +1709,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
         <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34">
         <v>394</v>
@@ -1734,13 +1723,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
         <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35">
         <v>411</v>
@@ -1748,13 +1737,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36">
         <v>367</v>
@@ -1762,13 +1751,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
         <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1776,13 +1765,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
         <v>92</v>
-      </c>
-      <c r="C38" t="s">
-        <v>93</v>
       </c>
       <c r="D38">
         <v>789</v>
@@ -1790,13 +1779,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39">
         <v>770</v>
@@ -1804,13 +1793,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D40">
         <v>759</v>
@@ -1818,13 +1807,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1832,13 +1821,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D42">
         <v>1059</v>
@@ -1846,13 +1835,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D43">
         <v>996</v>
@@ -1860,13 +1849,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
         <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44">
         <v>938</v>
@@ -1874,13 +1863,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1888,13 +1877,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
         <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D46">
         <v>1848</v>
@@ -1902,13 +1891,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
         <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D47">
         <v>1766</v>
@@ -1916,13 +1905,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" t="s">
         <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D48">
         <v>1697</v>
@@ -1930,13 +1919,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
         <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1944,13 +1933,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" t="s">
         <v>92</v>
-      </c>
-      <c r="C50" t="s">
-        <v>93</v>
       </c>
       <c r="D50">
         <v>632</v>
@@ -1958,13 +1947,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D51">
         <v>542</v>
@@ -1972,13 +1961,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D52">
         <v>525</v>
@@ -1986,13 +1975,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2000,13 +1989,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
         <v>23</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D54">
         <v>692</v>
@@ -2014,13 +2003,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" t="s">
         <v>23</v>
       </c>
       <c r="C55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D55">
         <v>665</v>
@@ -2028,13 +2017,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
         <v>23</v>
       </c>
       <c r="C56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D56">
         <v>684</v>
@@ -2042,13 +2031,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
         <v>23</v>
       </c>
       <c r="C57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2056,13 +2045,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D58">
         <v>1324</v>
@@ -2070,13 +2059,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
         <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D59">
         <v>1207</v>
@@ -2084,13 +2073,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
         <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D60">
         <v>1209</v>
@@ -2098,13 +2087,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
         <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2112,13 +2101,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" t="s">
         <v>92</v>
-      </c>
-      <c r="C62" t="s">
-        <v>93</v>
       </c>
       <c r="D62">
         <v>24461</v>
@@ -2126,13 +2115,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D63">
         <v>24782</v>
@@ -2140,13 +2129,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D64">
         <v>25157</v>
@@ -2154,13 +2143,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D65">
         <v>25525</v>
@@ -2168,13 +2157,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
         <v>23</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D66">
         <v>26003</v>
@@ -2182,13 +2171,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
         <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D67">
         <v>26496</v>
@@ -2196,13 +2185,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
         <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D68">
         <v>26952</v>
@@ -2210,13 +2199,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B69" t="s">
         <v>23</v>
       </c>
       <c r="C69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D69">
         <v>27384</v>
@@ -2224,13 +2213,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
         <v>22</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D70">
         <v>50464</v>
@@ -2238,13 +2227,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B71" t="s">
         <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D71">
         <v>51278</v>
@@ -2252,13 +2241,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B72" t="s">
         <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D72">
         <v>52109</v>
@@ -2266,13 +2255,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B73" t="s">
         <v>22</v>
       </c>
       <c r="C73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D73">
         <v>52909</v>
@@ -2280,13 +2269,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B74" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" t="s">
         <v>92</v>
-      </c>
-      <c r="C74" t="s">
-        <v>93</v>
       </c>
       <c r="D74">
         <v>24782</v>
@@ -2294,13 +2283,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D75">
         <v>25157</v>
@@ -2308,13 +2297,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D76">
         <v>25525</v>
@@ -2322,13 +2311,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2336,13 +2325,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B78" t="s">
         <v>23</v>
       </c>
       <c r="C78" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D78">
         <v>26496</v>
@@ -2350,13 +2339,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B79" t="s">
         <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D79">
         <v>26952</v>
@@ -2364,13 +2353,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B80" t="s">
         <v>23</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D80">
         <v>27384</v>
@@ -2378,13 +2367,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B81" t="s">
         <v>23</v>
       </c>
       <c r="C81" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2392,13 +2381,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B82" t="s">
         <v>22</v>
       </c>
       <c r="C82" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D82">
         <v>51278</v>
@@ -2406,13 +2395,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B83" t="s">
         <v>22</v>
       </c>
       <c r="C83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D83">
         <v>52109</v>
@@ -2420,13 +2409,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B84" t="s">
         <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D84">
         <v>52909</v>
@@ -2434,13 +2423,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B85" t="s">
         <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D85">
         <v>0</v>

</xml_diff>

<commit_message>
Rename sheet 'Data' to 'Data table'
Close #151
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AB6162-17F0-44B3-972B-0CBAAADE3109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC519E25-E054-49C3-9D4F-BB0C75BF033D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17475" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
     <sheet name="Variables" sheetId="1" r:id="rId2"/>
     <sheet name="Codelists" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="5" r:id="rId4"/>
+    <sheet name="Data table" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -408,9 +408,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -448,9 +448,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -483,26 +483,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,26 +518,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -730,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1239,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F35C8BB-E3B8-40CE-889D-1EA9058649D8}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rename source_data to data
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC519E25-E054-49C3-9D4F-BB0C75BF033D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5513CA7B-0939-4939-8C89-964C59DB83D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14625" yWindow="6885" windowWidth="20625" windowHeight="15090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
     <sheet name="Variables" sheetId="1" r:id="rId2"/>
     <sheet name="Codelists" sheetId="3" r:id="rId3"/>
-    <sheet name="Data table" sheetId="5" r:id="rId4"/>
+    <sheet name="Data" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>

<commit_message>
Rename source_data to data (#157)
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC519E25-E054-49C3-9D4F-BB0C75BF033D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5513CA7B-0939-4939-8C89-964C59DB83D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14625" yWindow="6885" windowWidth="20625" windowHeight="15090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
     <sheet name="Variables" sheetId="1" r:id="rId2"/>
     <sheet name="Codelists" sheetId="3" r:id="rId3"/>
-    <sheet name="Data table" sheetId="5" r:id="rId4"/>
+    <sheet name="Data" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>

<commit_message>
Check for ilegal values in Variables sheets
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF63897A-55F3-48DD-88CA-74F71A8D9F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD2BF49-BA44-4361-9418-4D47B701D460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="16995" windowHeight="31785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="31680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="97">
   <si>
     <t>type</t>
   </si>
@@ -31,9 +31,6 @@
     <t/>
   </si>
   <si>
-    <t>2MD</t>
-  </si>
-  <si>
     <t>antal</t>
   </si>
   <si>
@@ -310,16 +307,13 @@
     <t>pivot</t>
   </si>
   <si>
-    <t>figures</t>
-  </si>
-  <si>
-    <t>stub</t>
-  </si>
-  <si>
-    <t>heading</t>
-  </si>
-  <si>
     <t>order</t>
+  </si>
+  <si>
+    <t>STUB</t>
+  </si>
+  <si>
+    <t>HEADING</t>
   </si>
 </sst>
 </file>
@@ -711,23 +705,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3">
         <v>2000</v>
@@ -735,127 +729,127 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -863,7 +857,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -871,18 +865,18 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +893,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -915,42 +909,39 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -964,48 +955,42 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
@@ -1013,19 +998,19 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
@@ -1058,159 +1043,159 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1231,27 +1216,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
       </c>
       <c r="D2">
         <v>338</v>
@@ -1259,13 +1244,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3">
         <v>340</v>
@@ -1273,13 +1258,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>310</v>
@@ -1287,13 +1272,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1301,13 +1286,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <v>346</v>
@@ -1315,13 +1300,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7">
         <v>343</v>
@@ -1329,13 +1314,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8">
         <v>368</v>
@@ -1343,13 +1328,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1357,13 +1342,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10">
         <v>684</v>
@@ -1371,13 +1356,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11">
         <v>683</v>
@@ -1385,13 +1370,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12">
         <v>678</v>
@@ -1399,13 +1384,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1413,13 +1398,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
         <v>87</v>
-      </c>
-      <c r="C14" t="s">
-        <v>88</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1427,13 +1412,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1441,13 +1426,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1455,13 +1440,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1469,13 +1454,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -1483,13 +1468,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1497,13 +1482,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1511,13 +1496,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1525,13 +1510,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1539,13 +1524,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1553,13 +1538,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1567,13 +1552,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1581,13 +1566,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
         <v>87</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
       </c>
       <c r="D26">
         <v>175</v>
@@ -1595,13 +1580,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D27">
         <v>193</v>
@@ -1609,13 +1594,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D28">
         <v>176</v>
@@ -1623,13 +1608,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1637,13 +1622,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30">
         <v>219</v>
@@ -1651,13 +1636,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D31">
         <v>218</v>
@@ -1665,13 +1650,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32">
         <v>191</v>
@@ -1679,13 +1664,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1693,13 +1678,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D34">
         <v>394</v>
@@ -1707,13 +1692,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D35">
         <v>411</v>
@@ -1721,13 +1706,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D36">
         <v>367</v>
@@ -1735,13 +1720,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1749,13 +1734,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" t="s">
         <v>87</v>
-      </c>
-      <c r="C38" t="s">
-        <v>88</v>
       </c>
       <c r="D38">
         <v>789</v>
@@ -1763,13 +1748,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D39">
         <v>770</v>
@@ -1777,13 +1762,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D40">
         <v>759</v>
@@ -1791,13 +1776,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1805,13 +1790,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D42">
         <v>1059</v>
@@ -1819,13 +1804,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43">
         <v>996</v>
@@ -1833,13 +1818,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D44">
         <v>938</v>
@@ -1847,13 +1832,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1861,13 +1846,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D46">
         <v>1848</v>
@@ -1875,13 +1860,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D47">
         <v>1766</v>
@@ -1889,13 +1874,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D48">
         <v>1697</v>
@@ -1903,13 +1888,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1917,13 +1902,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
         <v>87</v>
-      </c>
-      <c r="C50" t="s">
-        <v>88</v>
       </c>
       <c r="D50">
         <v>632</v>
@@ -1931,13 +1916,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51">
         <v>542</v>
@@ -1945,13 +1930,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D52">
         <v>525</v>
@@ -1959,13 +1944,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1973,13 +1958,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D54">
         <v>692</v>
@@ -1987,13 +1972,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D55">
         <v>665</v>
@@ -2001,13 +1986,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D56">
         <v>684</v>
@@ -2015,13 +2000,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2029,13 +2014,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D58">
         <v>1324</v>
@@ -2043,13 +2028,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D59">
         <v>1207</v>
@@ -2057,13 +2042,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D60">
         <v>1209</v>
@@ -2071,13 +2056,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2085,13 +2070,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" t="s">
         <v>87</v>
-      </c>
-      <c r="C62" t="s">
-        <v>88</v>
       </c>
       <c r="D62">
         <v>24461</v>
@@ -2099,13 +2084,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D63">
         <v>24782</v>
@@ -2113,13 +2098,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D64">
         <v>25157</v>
@@ -2127,13 +2112,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D65">
         <v>25525</v>
@@ -2141,13 +2126,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66">
         <v>26003</v>
@@ -2155,13 +2140,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D67">
         <v>26496</v>
@@ -2169,13 +2154,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D68">
         <v>26952</v>
@@ -2183,13 +2168,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69">
         <v>27384</v>
@@ -2197,13 +2182,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D70">
         <v>50464</v>
@@ -2211,13 +2196,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D71">
         <v>51278</v>
@@ -2225,13 +2210,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D72">
         <v>52109</v>
@@ -2239,13 +2224,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D73">
         <v>52909</v>
@@ -2253,13 +2238,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C74" t="s">
         <v>87</v>
-      </c>
-      <c r="C74" t="s">
-        <v>88</v>
       </c>
       <c r="D74">
         <v>24782</v>
@@ -2267,13 +2252,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D75">
         <v>25157</v>
@@ -2281,13 +2266,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D76">
         <v>25525</v>
@@ -2295,13 +2280,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2309,13 +2294,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D78">
         <v>26496</v>
@@ -2323,13 +2308,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D79">
         <v>26952</v>
@@ -2337,13 +2322,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D80">
         <v>27384</v>
@@ -2351,13 +2336,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B81" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2365,13 +2350,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D82">
         <v>51278</v>
@@ -2379,13 +2364,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B83" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D83">
         <v>52109</v>
@@ -2393,13 +2378,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B84" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D84">
         <v>52909</v>
@@ -2407,13 +2392,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B85" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D85">
         <v>0</v>

</xml_diff>

<commit_message>
Set latin1 to default encoding, but add CODEPAGE=utf-8
Close #190
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37183AB1-05B4-4430-ADB6-0D9AAB6F5494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C8D869-8112-41C7-A50B-B5C2357919F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="17475" windowHeight="31785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="94">
   <si>
     <t>keyword</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>2000Q4</t>
+  </si>
+  <si>
+    <t>CODEPAGE</t>
+  </si>
+  <si>
+    <t>utf-8</t>
   </si>
 </sst>
 </file>
@@ -355,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:B12" totalsRowShown="0">
-  <autoFilter ref="A1:B12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:B13" totalsRowShown="0">
+  <autoFilter ref="A1:B13" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keyword"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="value"/>
@@ -699,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,6 +811,14 @@
       </c>
       <c r="B12" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>